<commit_message>
Fix rebase navbar on dev (2/2)
</commit_message>
<xml_diff>
--- a/doc/Gantt.xlsx
+++ b/doc/Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DF0549-991C-4F0B-89A5-908BAEF99347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D24B55-AE1F-4D0D-935B-81167EC0DFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-116" yWindow="-116" windowWidth="24917" windowHeight="13513" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>Créez un planning de projet dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>CRUD</t>
+  </si>
+  <si>
+    <t>Théo, Nicolas</t>
   </si>
 </sst>
 </file>
@@ -1938,8 +1941,8 @@
   <dimension ref="A1:AC38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2744,9 +2747,11 @@
       <c r="B19" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="42"/>
+      <c r="C19" s="42" t="s">
+        <v>56</v>
+      </c>
       <c r="D19" s="19">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="E19" s="65">
         <v>44797</v>
@@ -2786,9 +2791,11 @@
       <c r="B20" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="42"/>
+      <c r="C20" s="42" t="s">
+        <v>60</v>
+      </c>
       <c r="D20" s="19">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E20" s="65">
         <v>44797</v>
@@ -2825,9 +2832,11 @@
       <c r="B21" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="42"/>
+      <c r="C21" s="42" t="s">
+        <v>55</v>
+      </c>
       <c r="D21" s="19">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E21" s="65">
         <v>44797</v>
@@ -2867,9 +2876,11 @@
       <c r="B22" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="42"/>
+      <c r="C22" s="42" t="s">
+        <v>51</v>
+      </c>
       <c r="D22" s="19">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E22" s="65">
         <v>44802</v>
@@ -2942,9 +2953,11 @@
       <c r="B24" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="72"/>
+      <c r="C24" s="72" t="s">
+        <v>54</v>
+      </c>
       <c r="D24" s="73">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E24" s="74">
         <v>44799</v>
@@ -3061,7 +3074,7 @@
       </c>
       <c r="C27" s="72"/>
       <c r="D27" s="73">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E27" s="74">
         <v>44799</v>

</xml_diff>

<commit_message>
dev(navbar) : Add search pannel to navbar
</commit_message>
<xml_diff>
--- a/doc/Gantt.xlsx
+++ b/doc/Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D24B55-AE1F-4D0D-935B-81167EC0DFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415E3EDB-BE73-4012-8B7B-447CEFA45DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-116" yWindow="-116" windowWidth="24917" windowHeight="13513" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
   <si>
     <t>Créez un planning de projet dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -273,7 +273,7 @@
     <numFmt numFmtId="171" formatCode="d\ mmm\ yyyy;@"/>
     <numFmt numFmtId="172" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1940,12 +1940,12 @@
   </sheetPr>
   <dimension ref="A1:AC38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AP32" sqref="AP32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="31" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
@@ -1958,7 +1958,7 @@
     <col min="9" max="29" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:29" ht="30.05" customHeight="1">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" ht="30.05" customHeight="1">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="30.05" customHeight="1">
       <c r="A3" s="31" t="s">
         <v>2</v>
       </c>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="F3" s="89"/>
     </row>
-    <row r="4" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="30.05" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>3</v>
       </c>
@@ -2046,7 +2046,7 @@
       <c r="AB4" s="91"/>
       <c r="AC4" s="92"/>
     </row>
-    <row r="5" spans="1:29" s="79" customFormat="1" ht="14.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" s="79" customFormat="1" ht="14.95" customHeight="1">
       <c r="A5" s="78" t="s">
         <v>4</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>44815</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="87" customFormat="1" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" s="87" customFormat="1" ht="28.95" customHeight="1" thickBot="1">
       <c r="A6" s="83" t="s">
         <v>5</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>d</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="12.9" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" ht="12.9" hidden="1" customHeight="1" thickBot="1">
       <c r="A7" s="31" t="s">
         <v>6</v>
       </c>
@@ -2281,7 +2281,7 @@
       <c r="AB7" s="27"/>
       <c r="AC7" s="27"/>
     </row>
-    <row r="8" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A8" s="32" t="s">
         <v>7</v>
       </c>
@@ -2319,7 +2319,7 @@
       <c r="AB8" s="27"/>
       <c r="AC8" s="27"/>
     </row>
-    <row r="9" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A9" s="32" t="s">
         <v>8</v>
       </c>
@@ -2365,7 +2365,7 @@
       <c r="AB9" s="27"/>
       <c r="AC9" s="27"/>
     </row>
-    <row r="10" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A10" s="32" t="s">
         <v>9</v>
       </c>
@@ -2411,7 +2411,7 @@
       <c r="AB10" s="27"/>
       <c r="AC10" s="27"/>
     </row>
-    <row r="11" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A11" s="32"/>
       <c r="B11" s="46" t="s">
         <v>27</v>
@@ -2452,7 +2452,7 @@
       <c r="AB11" s="27"/>
       <c r="AC11" s="27"/>
     </row>
-    <row r="12" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A12" s="32" t="s">
         <v>10</v>
       </c>
@@ -2490,7 +2490,7 @@
       <c r="AB12" s="27"/>
       <c r="AC12" s="27"/>
     </row>
-    <row r="13" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A13" s="31"/>
       <c r="B13" s="47" t="s">
         <v>28</v>
@@ -2534,7 +2534,7 @@
       <c r="AB13" s="27"/>
       <c r="AC13" s="27"/>
     </row>
-    <row r="14" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A14" s="31"/>
       <c r="B14" s="47" t="s">
         <v>42</v>
@@ -2578,7 +2578,7 @@
       <c r="AB14" s="27"/>
       <c r="AC14" s="27"/>
     </row>
-    <row r="15" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A15" s="31"/>
       <c r="B15" s="47" t="s">
         <v>44</v>
@@ -2619,7 +2619,7 @@
       <c r="AB15" s="27"/>
       <c r="AC15" s="27"/>
     </row>
-    <row r="16" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A16" s="31"/>
       <c r="B16" s="47" t="s">
         <v>43</v>
@@ -2660,7 +2660,7 @@
       <c r="AB16" s="27"/>
       <c r="AC16" s="27"/>
     </row>
-    <row r="17" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A17" s="31"/>
       <c r="B17" s="47" t="s">
         <v>52</v>
@@ -2704,7 +2704,7 @@
       <c r="AB17" s="27"/>
       <c r="AC17" s="27"/>
     </row>
-    <row r="18" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A18" s="31" t="s">
         <v>11</v>
       </c>
@@ -2742,7 +2742,7 @@
       <c r="AB18" s="27"/>
       <c r="AC18" s="27"/>
     </row>
-    <row r="19" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A19" s="31"/>
       <c r="B19" s="48" t="s">
         <v>57</v>
@@ -2751,7 +2751,7 @@
         <v>56</v>
       </c>
       <c r="D19" s="19">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="E19" s="65">
         <v>44797</v>
@@ -2786,7 +2786,7 @@
       <c r="AB19" s="27"/>
       <c r="AC19" s="27"/>
     </row>
-    <row r="20" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A20" s="31"/>
       <c r="B20" s="48" t="s">
         <v>58</v>
@@ -2827,7 +2827,7 @@
       <c r="AB20" s="27"/>
       <c r="AC20" s="27"/>
     </row>
-    <row r="21" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A21" s="31"/>
       <c r="B21" s="77" t="s">
         <v>46</v>
@@ -2871,7 +2871,7 @@
       <c r="AB21" s="27"/>
       <c r="AC21" s="27"/>
     </row>
-    <row r="22" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A22" s="31"/>
       <c r="B22" s="48" t="s">
         <v>50</v>
@@ -2880,7 +2880,7 @@
         <v>51</v>
       </c>
       <c r="D22" s="19">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="E22" s="65">
         <v>44802</v>
@@ -2915,7 +2915,7 @@
       <c r="AB22" s="27"/>
       <c r="AC22" s="27"/>
     </row>
-    <row r="23" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A23" s="31"/>
       <c r="B23" s="67" t="s">
         <v>29</v>
@@ -2948,7 +2948,7 @@
       <c r="AB23" s="27"/>
       <c r="AC23" s="27"/>
     </row>
-    <row r="24" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A24" s="31"/>
       <c r="B24" s="71" t="s">
         <v>45</v>
@@ -2957,7 +2957,7 @@
         <v>54</v>
       </c>
       <c r="D24" s="73">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E24" s="74">
         <v>44799</v>
@@ -2989,14 +2989,16 @@
       <c r="AB24" s="27"/>
       <c r="AC24" s="27"/>
     </row>
-    <row r="25" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A25" s="31"/>
       <c r="B25" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="72"/>
+      <c r="C25" s="72" t="s">
+        <v>56</v>
+      </c>
       <c r="D25" s="73">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E25" s="74">
         <v>44798</v>
@@ -3028,7 +3030,7 @@
       <c r="AB25" s="27"/>
       <c r="AC25" s="27"/>
     </row>
-    <row r="26" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A26" s="31"/>
       <c r="B26" s="71" t="s">
         <v>48</v>
@@ -3067,14 +3069,14 @@
       <c r="AB26" s="27"/>
       <c r="AC26" s="27"/>
     </row>
-    <row r="27" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A27" s="31"/>
       <c r="B27" s="71" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="72"/>
       <c r="D27" s="73">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E27" s="74">
         <v>44799</v>
@@ -3106,7 +3108,7 @@
       <c r="AB27" s="27"/>
       <c r="AC27" s="27"/>
     </row>
-    <row r="28" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A28" s="31"/>
       <c r="B28" s="71" t="s">
         <v>47</v>
@@ -3145,7 +3147,7 @@
       <c r="AB28" s="27"/>
       <c r="AC28" s="27"/>
     </row>
-    <row r="29" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A29" s="31"/>
       <c r="B29" s="71" t="s">
         <v>49</v>
@@ -3184,7 +3186,7 @@
       <c r="AB29" s="27"/>
       <c r="AC29" s="27"/>
     </row>
-    <row r="30" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A30" s="31" t="s">
         <v>11</v>
       </c>
@@ -3222,7 +3224,7 @@
       <c r="AB30" s="27"/>
       <c r="AC30" s="27"/>
     </row>
-    <row r="31" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A31" s="31"/>
       <c r="B31" s="49" t="s">
         <v>32</v>
@@ -3264,7 +3266,7 @@
       <c r="AB31" s="27"/>
       <c r="AC31" s="27"/>
     </row>
-    <row r="32" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A32" s="31"/>
       <c r="B32" s="49" t="s">
         <v>33</v>
@@ -3306,7 +3308,7 @@
       <c r="AB32" s="27"/>
       <c r="AC32" s="27"/>
     </row>
-    <row r="33" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A33" s="31"/>
       <c r="B33" s="49" t="s">
         <v>41</v>
@@ -3348,7 +3350,7 @@
       <c r="AB33" s="27"/>
       <c r="AC33" s="27"/>
     </row>
-    <row r="34" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A34" s="31" t="s">
         <v>12</v>
       </c>
@@ -3384,7 +3386,7 @@
       <c r="AB34" s="27"/>
       <c r="AC34" s="27"/>
     </row>
-    <row r="35" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
       <c r="A35" s="32" t="s">
         <v>13</v>
       </c>
@@ -3422,14 +3424,14 @@
       <c r="AB35" s="29"/>
       <c r="AC35" s="29"/>
     </row>
-    <row r="36" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" ht="30.05" customHeight="1">
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" ht="30.05" customHeight="1">
       <c r="C37" s="8"/>
       <c r="F37" s="33"/>
     </row>
-    <row r="38" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" ht="30.05" customHeight="1">
       <c r="C38" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dev(Products) : Card animation
</commit_message>
<xml_diff>
--- a/doc/Gantt.xlsx
+++ b/doc/Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415E3EDB-BE73-4012-8B7B-447CEFA45DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948BE2E1-34DB-44E5-9CA8-A9A3B23CBA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-116" yWindow="-116" windowWidth="24917" windowHeight="13513" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>Créez un planning de projet dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -273,7 +273,7 @@
     <numFmt numFmtId="171" formatCode="d\ mmm\ yyyy;@"/>
     <numFmt numFmtId="172" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1940,12 +1940,12 @@
   </sheetPr>
   <dimension ref="A1:AC38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP32" sqref="AP32"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30.05" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="31" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
@@ -1958,7 +1958,7 @@
     <col min="9" max="29" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="30.05" customHeight="1">
+    <row r="1" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="30.05" customHeight="1">
+    <row r="2" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="30.05" customHeight="1">
+    <row r="3" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>2</v>
       </c>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="F3" s="89"/>
     </row>
-    <row r="4" spans="1:29" ht="30.05" customHeight="1">
+    <row r="4" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>3</v>
       </c>
@@ -2046,7 +2046,7 @@
       <c r="AB4" s="91"/>
       <c r="AC4" s="92"/>
     </row>
-    <row r="5" spans="1:29" s="79" customFormat="1" ht="14.95" customHeight="1">
+    <row r="5" spans="1:29" s="79" customFormat="1" ht="14.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="78" t="s">
         <v>4</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>44815</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="87" customFormat="1" ht="28.95" customHeight="1" thickBot="1">
+    <row r="6" spans="1:29" s="87" customFormat="1" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="83" t="s">
         <v>5</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>d</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="12.9" hidden="1" customHeight="1" thickBot="1">
+    <row r="7" spans="1:29" ht="12.9" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
         <v>6</v>
       </c>
@@ -2281,7 +2281,7 @@
       <c r="AB7" s="27"/>
       <c r="AC7" s="27"/>
     </row>
-    <row r="8" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="8" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
         <v>7</v>
       </c>
@@ -2319,7 +2319,7 @@
       <c r="AB8" s="27"/>
       <c r="AC8" s="27"/>
     </row>
-    <row r="9" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="9" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="32" t="s">
         <v>8</v>
       </c>
@@ -2365,7 +2365,7 @@
       <c r="AB9" s="27"/>
       <c r="AC9" s="27"/>
     </row>
-    <row r="10" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="10" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="32" t="s">
         <v>9</v>
       </c>
@@ -2411,7 +2411,7 @@
       <c r="AB10" s="27"/>
       <c r="AC10" s="27"/>
     </row>
-    <row r="11" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="11" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="32"/>
       <c r="B11" s="46" t="s">
         <v>27</v>
@@ -2452,7 +2452,7 @@
       <c r="AB11" s="27"/>
       <c r="AC11" s="27"/>
     </row>
-    <row r="12" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="12" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="32" t="s">
         <v>10</v>
       </c>
@@ -2490,7 +2490,7 @@
       <c r="AB12" s="27"/>
       <c r="AC12" s="27"/>
     </row>
-    <row r="13" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="13" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="31"/>
       <c r="B13" s="47" t="s">
         <v>28</v>
@@ -2534,7 +2534,7 @@
       <c r="AB13" s="27"/>
       <c r="AC13" s="27"/>
     </row>
-    <row r="14" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="14" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="31"/>
       <c r="B14" s="47" t="s">
         <v>42</v>
@@ -2578,7 +2578,7 @@
       <c r="AB14" s="27"/>
       <c r="AC14" s="27"/>
     </row>
-    <row r="15" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="15" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31"/>
       <c r="B15" s="47" t="s">
         <v>44</v>
@@ -2619,7 +2619,7 @@
       <c r="AB15" s="27"/>
       <c r="AC15" s="27"/>
     </row>
-    <row r="16" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="16" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="31"/>
       <c r="B16" s="47" t="s">
         <v>43</v>
@@ -2660,7 +2660,7 @@
       <c r="AB16" s="27"/>
       <c r="AC16" s="27"/>
     </row>
-    <row r="17" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="17" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="31"/>
       <c r="B17" s="47" t="s">
         <v>52</v>
@@ -2704,7 +2704,7 @@
       <c r="AB17" s="27"/>
       <c r="AC17" s="27"/>
     </row>
-    <row r="18" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="18" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="31" t="s">
         <v>11</v>
       </c>
@@ -2742,7 +2742,7 @@
       <c r="AB18" s="27"/>
       <c r="AC18" s="27"/>
     </row>
-    <row r="19" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="19" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="31"/>
       <c r="B19" s="48" t="s">
         <v>57</v>
@@ -2751,7 +2751,7 @@
         <v>56</v>
       </c>
       <c r="D19" s="19">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E19" s="65">
         <v>44797</v>
@@ -2786,7 +2786,7 @@
       <c r="AB19" s="27"/>
       <c r="AC19" s="27"/>
     </row>
-    <row r="20" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="20" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="31"/>
       <c r="B20" s="48" t="s">
         <v>58</v>
@@ -2795,7 +2795,7 @@
         <v>60</v>
       </c>
       <c r="D20" s="19">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E20" s="65">
         <v>44797</v>
@@ -2827,7 +2827,7 @@
       <c r="AB20" s="27"/>
       <c r="AC20" s="27"/>
     </row>
-    <row r="21" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="21" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="31"/>
       <c r="B21" s="77" t="s">
         <v>46</v>
@@ -2836,7 +2836,7 @@
         <v>55</v>
       </c>
       <c r="D21" s="19">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="E21" s="65">
         <v>44797</v>
@@ -2871,7 +2871,7 @@
       <c r="AB21" s="27"/>
       <c r="AC21" s="27"/>
     </row>
-    <row r="22" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="22" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="31"/>
       <c r="B22" s="48" t="s">
         <v>50</v>
@@ -2880,7 +2880,7 @@
         <v>51</v>
       </c>
       <c r="D22" s="19">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="E22" s="65">
         <v>44802</v>
@@ -2915,7 +2915,7 @@
       <c r="AB22" s="27"/>
       <c r="AC22" s="27"/>
     </row>
-    <row r="23" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="23" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="31"/>
       <c r="B23" s="67" t="s">
         <v>29</v>
@@ -2948,16 +2948,16 @@
       <c r="AB23" s="27"/>
       <c r="AC23" s="27"/>
     </row>
-    <row r="24" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="24" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="31"/>
       <c r="B24" s="71" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="72" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D24" s="73">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E24" s="74">
         <v>44799</v>
@@ -2989,16 +2989,16 @@
       <c r="AB24" s="27"/>
       <c r="AC24" s="27"/>
     </row>
-    <row r="25" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="25" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="31"/>
       <c r="B25" s="71" t="s">
         <v>59</v>
       </c>
       <c r="C25" s="72" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D25" s="73">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="E25" s="74">
         <v>44798</v>
@@ -3030,14 +3030,16 @@
       <c r="AB25" s="27"/>
       <c r="AC25" s="27"/>
     </row>
-    <row r="26" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="26" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="31"/>
       <c r="B26" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="72"/>
+      <c r="C26" s="72" t="s">
+        <v>51</v>
+      </c>
       <c r="D26" s="73">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E26" s="74">
         <v>44799</v>
@@ -3069,14 +3071,16 @@
       <c r="AB26" s="27"/>
       <c r="AC26" s="27"/>
     </row>
-    <row r="27" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="27" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="31"/>
       <c r="B27" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="72"/>
+      <c r="C27" s="72" t="s">
+        <v>51</v>
+      </c>
       <c r="D27" s="73">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="E27" s="74">
         <v>44799</v>
@@ -3108,7 +3112,7 @@
       <c r="AB27" s="27"/>
       <c r="AC27" s="27"/>
     </row>
-    <row r="28" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="28" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="31"/>
       <c r="B28" s="71" t="s">
         <v>47</v>
@@ -3147,7 +3151,7 @@
       <c r="AB28" s="27"/>
       <c r="AC28" s="27"/>
     </row>
-    <row r="29" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="29" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="31"/>
       <c r="B29" s="71" t="s">
         <v>49</v>
@@ -3186,7 +3190,7 @@
       <c r="AB29" s="27"/>
       <c r="AC29" s="27"/>
     </row>
-    <row r="30" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="30" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="31" t="s">
         <v>11</v>
       </c>
@@ -3224,7 +3228,7 @@
       <c r="AB30" s="27"/>
       <c r="AC30" s="27"/>
     </row>
-    <row r="31" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="31" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="31"/>
       <c r="B31" s="49" t="s">
         <v>32</v>
@@ -3266,7 +3270,7 @@
       <c r="AB31" s="27"/>
       <c r="AC31" s="27"/>
     </row>
-    <row r="32" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="32" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="31"/>
       <c r="B32" s="49" t="s">
         <v>33</v>
@@ -3308,14 +3312,16 @@
       <c r="AB32" s="27"/>
       <c r="AC32" s="27"/>
     </row>
-    <row r="33" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="33" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="31"/>
       <c r="B33" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="44"/>
+      <c r="C33" s="44" t="s">
+        <v>54</v>
+      </c>
       <c r="D33" s="22">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E33" s="66">
         <v>44799</v>
@@ -3350,7 +3356,7 @@
       <c r="AB33" s="27"/>
       <c r="AC33" s="27"/>
     </row>
-    <row r="34" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="34" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="31" t="s">
         <v>12</v>
       </c>
@@ -3386,7 +3392,7 @@
       <c r="AB34" s="27"/>
       <c r="AC34" s="27"/>
     </row>
-    <row r="35" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1">
+    <row r="35" spans="1:29" s="3" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="32" t="s">
         <v>13</v>
       </c>
@@ -3424,14 +3430,14 @@
       <c r="AB35" s="29"/>
       <c r="AC35" s="29"/>
     </row>
-    <row r="36" spans="1:29" ht="30.05" customHeight="1">
+    <row r="36" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:29" ht="30.05" customHeight="1">
+    <row r="37" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="8"/>
       <c r="F37" s="33"/>
     </row>
-    <row r="38" spans="1:29" ht="30.05" customHeight="1">
+    <row r="38" spans="1:29" ht="30.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C38" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dev(Refactor) : Update navbar active
</commit_message>
<xml_diff>
--- a/doc/Gantt.xlsx
+++ b/doc/Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948BE2E1-34DB-44E5-9CA8-A9A3B23CBA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B97B7A-259B-4C38-8EC5-D7517BFA5AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-116" yWindow="-116" windowWidth="24917" windowHeight="13513" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>Créez un planning de projet dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -1941,8 +1941,8 @@
   <dimension ref="A1:AC38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2836,7 +2836,7 @@
         <v>55</v>
       </c>
       <c r="D21" s="19">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E21" s="65">
         <v>44797</v>
@@ -2880,7 +2880,7 @@
         <v>51</v>
       </c>
       <c r="D22" s="19">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E22" s="65">
         <v>44802</v>
@@ -2998,7 +2998,7 @@
         <v>51</v>
       </c>
       <c r="D25" s="73">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E25" s="74">
         <v>44798</v>
@@ -3039,7 +3039,7 @@
         <v>51</v>
       </c>
       <c r="D26" s="73">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E26" s="74">
         <v>44799</v>
@@ -3080,7 +3080,7 @@
         <v>51</v>
       </c>
       <c r="D27" s="73">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E27" s="74">
         <v>44799</v>
@@ -3117,9 +3117,11 @@
       <c r="B28" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="72"/>
+      <c r="C28" s="72" t="s">
+        <v>53</v>
+      </c>
       <c r="D28" s="73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="74">
         <v>44802</v>

</xml_diff>